<commit_message>
Updated Vlookup and Hlookup files and included temp file
</commit_message>
<xml_diff>
--- a/vlookup_and_hlookup.xlsx
+++ b/vlookup_and_hlookup.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data Analytics\Excel\Day-12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analytics\Excel\Day-12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A64CA7-8111-4A74-95D9-FBA75F170EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7014E9B2-A51D-4BF9-BEA9-266D01F8B8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{1CAEC8E1-DBF7-47F7-A0EC-6B0593168D15}"/>
   </bookViews>
@@ -126,7 +126,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +148,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -179,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -187,12 +193,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,10 +526,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:15" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="8"/>
+      <c r="K4" s="5"/>
     </row>
     <row r="7" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D7" s="1" t="s">
@@ -772,10 +777,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D058EDD8-5DC2-48FC-9CCD-CFE170F7D74F}">
-  <dimension ref="D4:S19"/>
+  <dimension ref="D4:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -787,10 +792,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="I4" s="8" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="8"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="6"/>
     </row>
     <row r="7" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D7" s="1" t="s">
@@ -837,30 +844,30 @@
       </c>
     </row>
     <row r="8" spans="4:19" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="6" t="str">
+      <c r="E8" s="4" t="str">
         <f>HLOOKUP(E7,$M$7:$S$9,2,)</f>
         <v>automotive sq, near tp road, 4000001</v>
       </c>
-      <c r="F8" s="6" t="str">
+      <c r="F8" s="4" t="str">
         <f t="shared" ref="F8:J8" si="0">HLOOKUP(F7,$M$7:$S$9,2,)</f>
         <v>offline</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="4">
         <f t="shared" si="0"/>
         <v>5000</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="4">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="4">
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
@@ -1013,19 +1020,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="12:18" x14ac:dyDescent="0.3">
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="I4:J4"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>